<commit_message>
dodanie odnosnikow do components PSCP I PSAPT dodanie sarch by SAP ID i Customer dodanie punktu granicznego - classification nieudana proba dodania classification chart
</commit_message>
<xml_diff>
--- a/src/main/resources/002.xlsx
+++ b/src/main/resources/002.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\olek\JAVA_DRUGIE_PODEJSCIE\SPRING\H2\SPRING_08_MYSQL_COMPANY\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{54C4AACA-1F29-405D-BB03-06907D94E269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033A0A91-BD81-4F82-94CA-9781AEBCACB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="002" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,22 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'002'!$A$4:$U$1111</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Arkusz1!$A$2:$E$151</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7987" uniqueCount="1668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8137" uniqueCount="1668">
   <si>
     <t>id</t>
   </si>
@@ -5034,7 +5044,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5983,10 +5993,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:W1111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:P1111"/>
     </sheetView>
   </sheetViews>
@@ -68045,7 +68055,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:U1111"/>
+  <autoFilter ref="A4:U1111" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -68053,16 +68063,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J151"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:Q151"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="L153" sqref="L153"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:Q151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -68085,8 +68095,26 @@
         <f>CEILING(E2,2)</f>
         <v>98</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f ca="1">RAND()</f>
+        <v>0.6195534784394946</v>
+      </c>
+      <c r="N2">
+        <f ca="1">M2*E2</f>
+        <v>60.71624088707047</v>
+      </c>
+      <c r="O2">
+        <f ca="1">CEILING(N2,1)</f>
+        <v>61</v>
+      </c>
+      <c r="P2">
+        <v>45</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -68109,8 +68137,26 @@
         <f t="shared" ref="J3:J65" si="0">CEILING(E3,2)</f>
         <v>98</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f t="shared" ref="M3:M66" ca="1" si="1">RAND()</f>
+        <v>0.95353199910326325</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N66" ca="1" si="2">M3*E3</f>
+        <v>93.4461359121198</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O66" ca="1" si="3">CEILING(N3,1)</f>
+        <v>94</v>
+      </c>
+      <c r="P3">
+        <v>53</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -68133,8 +68179,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.26619903696625846</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ca="1" si="2"/>
+        <v>26.619903696625848</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ca="1" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="P4">
+        <v>6</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -68157,8 +68221,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.53732478040475573</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ca="1" si="2"/>
+        <v>52.657828479666058</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ca="1" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="P5">
+        <v>77</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -68181,8 +68263,26 @@
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.53574778936851786</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ca="1" si="2"/>
+        <v>43.931318728218464</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ca="1" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="P6">
+        <v>58</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -68205,8 +68305,26 @@
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.37087957332471122</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ca="1" si="2"/>
+        <v>27.445088426028629</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ca="1" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="P7">
+        <v>7</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -68229,8 +68347,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.12618769787633233</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ca="1" si="2"/>
+        <v>12.618769787633234</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ca="1" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="P8">
+        <v>38</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -68253,8 +68389,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.52431294292881292</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ca="1" si="2"/>
+        <v>51.382668407023665</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ca="1" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="P9">
+        <v>33</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -68277,8 +68431,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.37446512630044748</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ca="1" si="2"/>
+        <v>36.697582377443851</v>
+      </c>
+      <c r="O10">
+        <f t="shared" ca="1" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="P10">
+        <v>16</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -68301,8 +68473,26 @@
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.15012837860327499</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ca="1" si="2"/>
+        <v>12.911040559881648</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ca="1" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="P11">
+        <v>36</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -68325,8 +68515,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.75558597096737079</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ca="1" si="2"/>
+        <v>74.04742515480234</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ca="1" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="P12">
+        <v>54</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -68349,8 +68557,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.61194748013821809</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.970853053545376</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ca="1" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="P13">
+        <v>97</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -68373,8 +68599,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.62743723509313731</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ca="1" si="2"/>
+        <v>61.488849039127459</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ca="1" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="P14">
+        <v>55</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -68397,8 +68641,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.75038952363344702</v>
+      </c>
+      <c r="N15">
+        <f t="shared" ca="1" si="2"/>
+        <v>73.538173316077803</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ca="1" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="P15">
+        <v>32</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -68421,8 +68683,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.59120795479022081</v>
+      </c>
+      <c r="N16">
+        <f t="shared" ca="1" si="2"/>
+        <v>57.938379569441636</v>
+      </c>
+      <c r="O16">
+        <f t="shared" ca="1" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="P16">
+        <v>28</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -68445,8 +68725,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.20369248538656204</v>
+      </c>
+      <c r="N17">
+        <f t="shared" ca="1" si="2"/>
+        <v>20.369248538656205</v>
+      </c>
+      <c r="O17">
+        <f t="shared" ca="1" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -68469,8 +68767,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.36169591255654487</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ca="1" si="2"/>
+        <v>35.446199430541398</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ca="1" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="P18">
+        <v>76</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -68493,8 +68809,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.54396502874989305</v>
+      </c>
+      <c r="N19">
+        <f t="shared" ca="1" si="2"/>
+        <v>53.308572817489519</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ca="1" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="P19">
+        <v>48</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -68517,8 +68851,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.50791682190059662</v>
+      </c>
+      <c r="N20">
+        <f t="shared" ca="1" si="2"/>
+        <v>49.775848546258466</v>
+      </c>
+      <c r="O20">
+        <f t="shared" ca="1" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="P20">
+        <v>29</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -68541,8 +68893,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.28015925541745623</v>
+      </c>
+      <c r="N21">
+        <f t="shared" ca="1" si="2"/>
+        <v>27.455607030910709</v>
+      </c>
+      <c r="O21">
+        <f t="shared" ca="1" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="P21">
+        <v>21</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -68565,8 +68935,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.79271748589000601</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ca="1" si="2"/>
+        <v>79.271748589000595</v>
+      </c>
+      <c r="O22">
+        <f t="shared" ca="1" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="P22">
+        <v>60</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -68589,8 +68977,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.66866219492159995</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ca="1" si="2"/>
+        <v>65.528895102316795</v>
+      </c>
+      <c r="O23">
+        <f t="shared" ca="1" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="P23">
+        <v>53</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -68613,8 +69019,26 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.89539549349013181</v>
+      </c>
+      <c r="N24">
+        <f t="shared" ca="1" si="2"/>
+        <v>84.167176388072392</v>
+      </c>
+      <c r="O24">
+        <f t="shared" ca="1" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="P24">
+        <v>52</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -68637,8 +69061,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.29377236859081335</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ca="1" si="2"/>
+        <v>28.789692121899709</v>
+      </c>
+      <c r="O25">
+        <f t="shared" ca="1" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="P25">
+        <v>32</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -68661,8 +69103,26 @@
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.64715608381749368</v>
+      </c>
+      <c r="N26">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.538359711209417</v>
+      </c>
+      <c r="O26">
+        <f t="shared" ca="1" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="P26">
+        <v>42</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -68685,8 +69145,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.77014486154946338</v>
+      </c>
+      <c r="N27">
+        <f t="shared" ca="1" si="2"/>
+        <v>75.474196431847417</v>
+      </c>
+      <c r="O27">
+        <f t="shared" ca="1" si="3"/>
+        <v>76</v>
+      </c>
+      <c r="P27">
+        <v>49</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -68709,8 +69187,26 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.68457362389229548</v>
+      </c>
+      <c r="N28">
+        <f t="shared" ca="1" si="2"/>
+        <v>64.34992064587577</v>
+      </c>
+      <c r="O28">
+        <f t="shared" ca="1" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="P28">
+        <v>2</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -68733,8 +69229,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.6194288962443979</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ca="1" si="2"/>
+        <v>60.704031831950992</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ca="1" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="P29">
+        <v>43</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -68757,8 +69271,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.42969948802330937</v>
+      </c>
+      <c r="N30">
+        <f t="shared" ca="1" si="2"/>
+        <v>42.11054982628432</v>
+      </c>
+      <c r="O30">
+        <f t="shared" ca="1" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="P30">
+        <v>10</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -68781,8 +69313,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.18556146191200051</v>
+      </c>
+      <c r="N31">
+        <f t="shared" ca="1" si="2"/>
+        <v>18.185023267376049</v>
+      </c>
+      <c r="O31">
+        <f t="shared" ca="1" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="P31">
+        <v>98</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -68805,8 +69355,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.84335679137707198</v>
+      </c>
+      <c r="N32">
+        <f t="shared" ca="1" si="2"/>
+        <v>82.648965554953051</v>
+      </c>
+      <c r="O32">
+        <f t="shared" ca="1" si="3"/>
+        <v>83</v>
+      </c>
+      <c r="P32">
+        <v>92</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -68829,8 +69397,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.74010593954753356</v>
+      </c>
+      <c r="N33">
+        <f t="shared" ca="1" si="2"/>
+        <v>74.010593954753361</v>
+      </c>
+      <c r="O33">
+        <f t="shared" ca="1" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="P33">
+        <v>69</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -68853,8 +69439,26 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.41449046268385992</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ca="1" si="2"/>
+        <v>38.962103492282836</v>
+      </c>
+      <c r="O34">
+        <f t="shared" ca="1" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="P34">
+        <v>69</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -68877,8 +69481,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.23222210411191124</v>
+      </c>
+      <c r="N35">
+        <f t="shared" ca="1" si="2"/>
+        <v>23.222210411191124</v>
+      </c>
+      <c r="O35">
+        <f t="shared" ca="1" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="P35">
+        <v>9</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -68901,8 +69523,26 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.46994856089116477</v>
+      </c>
+      <c r="N36">
+        <f t="shared" ca="1" si="2"/>
+        <v>44.175164723769491</v>
+      </c>
+      <c r="O36">
+        <f t="shared" ca="1" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="P36">
+        <v>21</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -68925,8 +69565,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.3457198075213284E-2</v>
+      </c>
+      <c r="N37">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.3457198075213284</v>
+      </c>
+      <c r="O37">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="P37">
+        <v>78</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -68949,8 +69607,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.49402085356958214</v>
+      </c>
+      <c r="N38">
+        <f t="shared" ca="1" si="2"/>
+        <v>48.41404364981905</v>
+      </c>
+      <c r="O38">
+        <f t="shared" ca="1" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="P38">
+        <v>3</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -68973,8 +69649,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.93470681507414788</v>
+      </c>
+      <c r="N39">
+        <f t="shared" ca="1" si="2"/>
+        <v>91.601267877266494</v>
+      </c>
+      <c r="O39">
+        <f t="shared" ca="1" si="3"/>
+        <v>92</v>
+      </c>
+      <c r="P39">
+        <v>21</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -68997,8 +69691,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.26086466255407703</v>
+      </c>
+      <c r="N40">
+        <f t="shared" ca="1" si="2"/>
+        <v>26.086466255407704</v>
+      </c>
+      <c r="O40">
+        <f t="shared" ca="1" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="P40">
+        <v>36</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -69021,8 +69733,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.82482241792006283</v>
+      </c>
+      <c r="N41">
+        <f t="shared" ca="1" si="2"/>
+        <v>82.482241792006278</v>
+      </c>
+      <c r="O41">
+        <f t="shared" ca="1" si="3"/>
+        <v>83</v>
+      </c>
+      <c r="P41">
+        <v>14</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -69045,8 +69775,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.86466786825308306</v>
+      </c>
+      <c r="N42">
+        <f t="shared" ca="1" si="2"/>
+        <v>84.737451088802146</v>
+      </c>
+      <c r="O42">
+        <f t="shared" ca="1" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="P42">
+        <v>96</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -69069,8 +69817,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.46696944750290348</v>
+      </c>
+      <c r="N43">
+        <f t="shared" ca="1" si="2"/>
+        <v>46.696944750290349</v>
+      </c>
+      <c r="O43">
+        <f t="shared" ca="1" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="P43">
+        <v>41</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -69093,8 +69859,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.64595269545259593</v>
+      </c>
+      <c r="N44">
+        <f t="shared" ca="1" si="2"/>
+        <v>63.303364154354398</v>
+      </c>
+      <c r="O44">
+        <f t="shared" ca="1" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="P44">
+        <v>57</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -69117,8 +69901,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M45">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.50323042793805395</v>
+      </c>
+      <c r="N45">
+        <f t="shared" ca="1" si="2"/>
+        <v>49.316581937929286</v>
+      </c>
+      <c r="O45">
+        <f t="shared" ca="1" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="P45">
+        <v>71</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -69141,8 +69943,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M46">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.35923506793107252</v>
+      </c>
+      <c r="N46">
+        <f t="shared" ca="1" si="2"/>
+        <v>35.20503665724511</v>
+      </c>
+      <c r="O46">
+        <f t="shared" ca="1" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="P46">
+        <v>91</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -69165,8 +69985,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.6374711525260971</v>
+      </c>
+      <c r="N47">
+        <f t="shared" ca="1" si="2"/>
+        <v>62.472172947557517</v>
+      </c>
+      <c r="O47">
+        <f t="shared" ca="1" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="P47">
+        <v>30</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -69189,8 +70027,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.19793950414435979</v>
+      </c>
+      <c r="N48">
+        <f t="shared" ca="1" si="2"/>
+        <v>19.39807140614726</v>
+      </c>
+      <c r="O48">
+        <f t="shared" ca="1" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="P48">
+        <v>70</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -69213,8 +70069,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M49">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.46388858072840378</v>
+      </c>
+      <c r="N49">
+        <f t="shared" ca="1" si="2"/>
+        <v>45.461080911383569</v>
+      </c>
+      <c r="O49">
+        <f t="shared" ca="1" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="P49">
+        <v>22</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -69237,8 +70111,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M50">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.36596739178884419</v>
+      </c>
+      <c r="N50">
+        <f t="shared" ca="1" si="2"/>
+        <v>35.864804395306727</v>
+      </c>
+      <c r="O50">
+        <f t="shared" ca="1" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="P50">
+        <v>87</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -69261,8 +70153,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M51">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.6884715287318971</v>
+      </c>
+      <c r="N51">
+        <f t="shared" ca="1" si="2"/>
+        <v>67.470209815725909</v>
+      </c>
+      <c r="O51">
+        <f t="shared" ca="1" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="P51">
+        <v>50</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -69285,8 +70195,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M52">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.83624952303641065</v>
+      </c>
+      <c r="N52">
+        <f t="shared" ca="1" si="2"/>
+        <v>83.624952303641066</v>
+      </c>
+      <c r="O52">
+        <f t="shared" ca="1" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="P52">
+        <v>29</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -69309,8 +70237,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M53">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.16333312357038898</v>
+      </c>
+      <c r="N53">
+        <f t="shared" ca="1" si="2"/>
+        <v>16.006646109898121</v>
+      </c>
+      <c r="O53">
+        <f t="shared" ca="1" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="P53">
+        <v>3</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -69333,8 +70279,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M54">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.92130851865686347</v>
+      </c>
+      <c r="N54">
+        <f t="shared" ca="1" si="2"/>
+        <v>90.288234828372623</v>
+      </c>
+      <c r="O54">
+        <f t="shared" ca="1" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="P54">
+        <v>59</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -69357,8 +70321,26 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M55">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9329447241387987</v>
+      </c>
+      <c r="N55">
+        <f t="shared" ca="1" si="2"/>
+        <v>87.696804069047076</v>
+      </c>
+      <c r="O55">
+        <f t="shared" ca="1" si="3"/>
+        <v>88</v>
+      </c>
+      <c r="P55">
+        <v>74</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -69381,8 +70363,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M56">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.565868467547987E-2</v>
+      </c>
+      <c r="N56">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4145510981970268</v>
+      </c>
+      <c r="O56">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="P56">
+        <v>68</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -69405,8 +70405,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M57">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.18752848727127236</v>
+      </c>
+      <c r="N57">
+        <f t="shared" ca="1" si="2"/>
+        <v>18.377791752584692</v>
+      </c>
+      <c r="O57">
+        <f t="shared" ca="1" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="P57">
+        <v>8</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -69429,8 +70447,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M58">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.52028074025383786</v>
+      </c>
+      <c r="N58">
+        <f t="shared" ca="1" si="2"/>
+        <v>50.987512544876111</v>
+      </c>
+      <c r="O58">
+        <f t="shared" ca="1" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="P58">
+        <v>22</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -69453,8 +70489,26 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M59">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.30764577230294221</v>
+      </c>
+      <c r="N59">
+        <f t="shared" ca="1" si="2"/>
+        <v>28.918702596476567</v>
+      </c>
+      <c r="O59">
+        <f t="shared" ca="1" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="P59">
+        <v>16</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -69477,8 +70531,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M60">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.30889116653662818</v>
+      </c>
+      <c r="N60">
+        <f t="shared" ca="1" si="2"/>
+        <v>30.889116653662818</v>
+      </c>
+      <c r="O60">
+        <f t="shared" ca="1" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="P60">
+        <v>99</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -69501,8 +70573,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M61">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.54670640644297019</v>
+      </c>
+      <c r="N61">
+        <f t="shared" ca="1" si="2"/>
+        <v>54.670640644297016</v>
+      </c>
+      <c r="O61">
+        <f t="shared" ca="1" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="P61">
+        <v>63</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -69525,8 +70615,26 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M62">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.85075762954122536</v>
+      </c>
+      <c r="N62">
+        <f t="shared" ca="1" si="2"/>
+        <v>85.075762954122538</v>
+      </c>
+      <c r="O62">
+        <f t="shared" ca="1" si="3"/>
+        <v>86</v>
+      </c>
+      <c r="P62">
+        <v>4</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -69549,8 +70657,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M63">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.66357827738099573</v>
+      </c>
+      <c r="N63">
+        <f t="shared" ca="1" si="2"/>
+        <v>65.030671183337574</v>
+      </c>
+      <c r="O63">
+        <f t="shared" ca="1" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="P63">
+        <v>37</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -69573,8 +70699,26 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M64">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.31947761280907361</v>
+      </c>
+      <c r="N64">
+        <f t="shared" ca="1" si="2"/>
+        <v>31.308806055289214</v>
+      </c>
+      <c r="O64">
+        <f t="shared" ca="1" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="P64">
+        <v>70</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -69597,8 +70741,26 @@
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M65">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.5840840438519685E-2</v>
+      </c>
+      <c r="N65">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.5223122777126932</v>
+      </c>
+      <c r="O65">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="P65">
+        <v>49</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -69618,11 +70780,29 @@
         <v>20</v>
       </c>
       <c r="J66">
-        <f t="shared" ref="J66:J128" si="1">CEILING(E66,2)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J66:J128" si="4">CEILING(E66,2)</f>
+        <v>100</v>
+      </c>
+      <c r="M66">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.73722490288598774</v>
+      </c>
+      <c r="N66">
+        <f t="shared" ca="1" si="2"/>
+        <v>73.722490288598777</v>
+      </c>
+      <c r="O66">
+        <f t="shared" ca="1" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="P66">
+        <v>65</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -69642,11 +70822,29 @@
         <v>51</v>
       </c>
       <c r="J67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M67">
+        <f t="shared" ref="M67:M130" ca="1" si="5">RAND()</f>
+        <v>4.9713815759638846E-2</v>
+      </c>
+      <c r="N67">
+        <f t="shared" ref="N67:N130" ca="1" si="6">M67*E67</f>
+        <v>4.6730986814060511</v>
+      </c>
+      <c r="O67">
+        <f t="shared" ref="O67:O130" ca="1" si="7">CEILING(N67,1)</f>
+        <v>5</v>
+      </c>
+      <c r="P67">
+        <v>74</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -69666,11 +70864,29 @@
         <v>51</v>
       </c>
       <c r="J68">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M68">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.57171665777662017</v>
+      </c>
+      <c r="N68">
+        <f t="shared" ca="1" si="6"/>
+        <v>56.028232462108775</v>
+      </c>
+      <c r="O68">
+        <f t="shared" ca="1" si="7"/>
+        <v>57</v>
+      </c>
+      <c r="P68">
+        <v>75</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -69690,11 +70906,29 @@
         <v>51</v>
       </c>
       <c r="J69">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M69">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.29044265366743915</v>
+      </c>
+      <c r="N69">
+        <f t="shared" ca="1" si="6"/>
+        <v>28.463380059409037</v>
+      </c>
+      <c r="O69">
+        <f t="shared" ca="1" si="7"/>
+        <v>29</v>
+      </c>
+      <c r="P69">
+        <v>51</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -69714,11 +70948,29 @@
         <v>20</v>
       </c>
       <c r="J70">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M70">
+        <f t="shared" ca="1" si="5"/>
+        <v>6.8395362416462602E-2</v>
+      </c>
+      <c r="N70">
+        <f t="shared" ca="1" si="6"/>
+        <v>6.7027455168133354</v>
+      </c>
+      <c r="O70">
+        <f t="shared" ca="1" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="P70">
+        <v>80</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -69738,11 +70990,29 @@
         <v>51</v>
       </c>
       <c r="J71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M71">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.38644771411433809</v>
+      </c>
+      <c r="N71">
+        <f t="shared" ca="1" si="6"/>
+        <v>36.326085126747778</v>
+      </c>
+      <c r="O71">
+        <f t="shared" ca="1" si="7"/>
+        <v>37</v>
+      </c>
+      <c r="P71">
+        <v>73</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -69762,11 +71032,29 @@
         <v>51</v>
       </c>
       <c r="J72">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M72">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.44319790642375867</v>
+      </c>
+      <c r="N72">
+        <f t="shared" ca="1" si="6"/>
+        <v>43.433394829528346</v>
+      </c>
+      <c r="O72">
+        <f t="shared" ca="1" si="7"/>
+        <v>44</v>
+      </c>
+      <c r="P72">
+        <v>64</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -69786,11 +71074,29 @@
         <v>51</v>
       </c>
       <c r="J73">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M73">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.51477539297352493</v>
+      </c>
+      <c r="N73">
+        <f t="shared" ca="1" si="6"/>
+        <v>50.447988511405441</v>
+      </c>
+      <c r="O73">
+        <f t="shared" ca="1" si="7"/>
+        <v>51</v>
+      </c>
+      <c r="P73">
+        <v>59</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -69810,11 +71116,29 @@
         <v>20</v>
       </c>
       <c r="J74">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M74">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.18948234857726021</v>
+      </c>
+      <c r="N74">
+        <f t="shared" ca="1" si="6"/>
+        <v>18.569270160571499</v>
+      </c>
+      <c r="O74">
+        <f t="shared" ca="1" si="7"/>
+        <v>19</v>
+      </c>
+      <c r="P74">
+        <v>33</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -69834,11 +71158,29 @@
         <v>20</v>
       </c>
       <c r="J75">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M75">
+        <f t="shared" ca="1" si="5"/>
+        <v>7.6992341747156634E-2</v>
+      </c>
+      <c r="N75">
+        <f t="shared" ca="1" si="6"/>
+        <v>7.5452494912213499</v>
+      </c>
+      <c r="O75">
+        <f t="shared" ca="1" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="P75">
+        <v>16</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -69858,11 +71200,29 @@
         <v>20</v>
       </c>
       <c r="J76">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="M76">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.2000384172303874</v>
+      </c>
+      <c r="N76">
+        <f t="shared" ca="1" si="6"/>
+        <v>20.00384172303874</v>
+      </c>
+      <c r="O76">
+        <f t="shared" ca="1" si="7"/>
+        <v>21</v>
+      </c>
+      <c r="P76">
+        <v>78</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -69882,11 +71242,29 @@
         <v>20</v>
       </c>
       <c r="J77">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M77">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.42493717020901389</v>
+      </c>
+      <c r="N77">
+        <f t="shared" ca="1" si="6"/>
+        <v>41.64384268048336</v>
+      </c>
+      <c r="O77">
+        <f t="shared" ca="1" si="7"/>
+        <v>42</v>
+      </c>
+      <c r="P77">
+        <v>37</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -69906,11 +71284,29 @@
         <v>20</v>
       </c>
       <c r="J78">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M78">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.53238031626722682</v>
+      </c>
+      <c r="N78">
+        <f t="shared" ca="1" si="6"/>
+        <v>52.173270994188229</v>
+      </c>
+      <c r="O78">
+        <f t="shared" ca="1" si="7"/>
+        <v>53</v>
+      </c>
+      <c r="P78">
+        <v>20</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -69930,11 +71326,29 @@
         <v>51</v>
       </c>
       <c r="J79">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M79">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.95297528899001238</v>
+      </c>
+      <c r="N79">
+        <f t="shared" ca="1" si="6"/>
+        <v>93.391578321021214</v>
+      </c>
+      <c r="O79">
+        <f t="shared" ca="1" si="7"/>
+        <v>94</v>
+      </c>
+      <c r="P79">
+        <v>11</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -69954,11 +71368,29 @@
         <v>20</v>
       </c>
       <c r="J80">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M80">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.67311368509204406</v>
+      </c>
+      <c r="N80">
+        <f t="shared" ca="1" si="6"/>
+        <v>65.965141139020318</v>
+      </c>
+      <c r="O80">
+        <f t="shared" ca="1" si="7"/>
+        <v>66</v>
+      </c>
+      <c r="P80">
+        <v>6</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -69978,11 +71410,29 @@
         <v>51</v>
       </c>
       <c r="J81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M81">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.5147716723514385</v>
+      </c>
+      <c r="N81">
+        <f t="shared" ca="1" si="6"/>
+        <v>49.418080545738093</v>
+      </c>
+      <c r="O81">
+        <f t="shared" ca="1" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="P81">
+        <v>49</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -70002,11 +71452,29 @@
         <v>51</v>
       </c>
       <c r="J82">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M82">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.7302142539151556</v>
+      </c>
+      <c r="N82">
+        <f t="shared" ca="1" si="6"/>
+        <v>71.560996883685249</v>
+      </c>
+      <c r="O82">
+        <f t="shared" ca="1" si="7"/>
+        <v>72</v>
+      </c>
+      <c r="P82">
+        <v>22</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -70026,11 +71494,29 @@
         <v>20</v>
       </c>
       <c r="J83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M83">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.91814601503619286</v>
+      </c>
+      <c r="N83">
+        <f t="shared" ca="1" si="6"/>
+        <v>33.053256541302943</v>
+      </c>
+      <c r="O83">
+        <f t="shared" ca="1" si="7"/>
+        <v>34</v>
+      </c>
+      <c r="P83">
+        <v>29</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -70050,11 +71536,29 @@
         <v>20</v>
       </c>
       <c r="J84">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M84">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.27120668611684573</v>
+      </c>
+      <c r="N84">
+        <f t="shared" ca="1" si="6"/>
+        <v>26.578255239450883</v>
+      </c>
+      <c r="O84">
+        <f t="shared" ca="1" si="7"/>
+        <v>27</v>
+      </c>
+      <c r="P84">
+        <v>2</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -70074,11 +71578,29 @@
         <v>20</v>
       </c>
       <c r="J85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M85">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.3676351251914407</v>
+      </c>
+      <c r="N85">
+        <f t="shared" ca="1" si="6"/>
+        <v>34.557701767995425</v>
+      </c>
+      <c r="O85">
+        <f t="shared" ca="1" si="7"/>
+        <v>35</v>
+      </c>
+      <c r="P85">
+        <v>19</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -70098,11 +71620,29 @@
         <v>20</v>
       </c>
       <c r="J86">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M86">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.983830010335863E-3</v>
+      </c>
+      <c r="N86">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.19441534101291458</v>
+      </c>
+      <c r="O86">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="P86">
+        <v>97</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -70122,11 +71662,29 @@
         <v>20</v>
       </c>
       <c r="J87">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M87">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.34945827827784792</v>
+      </c>
+      <c r="N87">
+        <f t="shared" ca="1" si="6"/>
+        <v>34.246911271229095</v>
+      </c>
+      <c r="O87">
+        <f t="shared" ca="1" si="7"/>
+        <v>35</v>
+      </c>
+      <c r="P87">
+        <v>58</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -70146,11 +71704,29 @@
         <v>51</v>
       </c>
       <c r="J88">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M88">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.52141680977291227</v>
+      </c>
+      <c r="N88">
+        <f t="shared" ca="1" si="6"/>
+        <v>51.098847357745406</v>
+      </c>
+      <c r="O88">
+        <f t="shared" ca="1" si="7"/>
+        <v>52</v>
+      </c>
+      <c r="P88">
+        <v>30</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -70170,11 +71746,29 @@
         <v>51</v>
       </c>
       <c r="J89">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M89">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.62073362785558572</v>
+      </c>
+      <c r="N89">
+        <f t="shared" ca="1" si="6"/>
+        <v>60.831895529847401</v>
+      </c>
+      <c r="O89">
+        <f t="shared" ca="1" si="7"/>
+        <v>61</v>
+      </c>
+      <c r="P89">
+        <v>30</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -70194,11 +71788,29 @@
         <v>20</v>
       </c>
       <c r="J90">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M90">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.74604420147547335</v>
+      </c>
+      <c r="N90">
+        <f t="shared" ca="1" si="6"/>
+        <v>73.112331744596389</v>
+      </c>
+      <c r="O90">
+        <f t="shared" ca="1" si="7"/>
+        <v>74</v>
+      </c>
+      <c r="P90">
+        <v>16</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -70218,11 +71830,29 @@
         <v>20</v>
       </c>
       <c r="J91">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M91">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.9002187884754829E-2</v>
+      </c>
+      <c r="N91">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.8622144127059732</v>
+      </c>
+      <c r="O91">
+        <f t="shared" ca="1" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="P91">
+        <v>57</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -70242,11 +71872,29 @@
         <v>51</v>
       </c>
       <c r="J92">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M92">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.98317082441626769</v>
+      </c>
+      <c r="N92">
+        <f t="shared" ca="1" si="6"/>
+        <v>96.350740792794227</v>
+      </c>
+      <c r="O92">
+        <f t="shared" ca="1" si="7"/>
+        <v>97</v>
+      </c>
+      <c r="P92">
+        <v>62</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -70266,11 +71914,29 @@
         <v>51</v>
       </c>
       <c r="J93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M93">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.74724995868041022</v>
+      </c>
+      <c r="N93">
+        <f t="shared" ca="1" si="6"/>
+        <v>70.241496115958554</v>
+      </c>
+      <c r="O93">
+        <f t="shared" ca="1" si="7"/>
+        <v>71</v>
+      </c>
+      <c r="P93">
+        <v>43</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -70290,11 +71956,29 @@
         <v>51</v>
       </c>
       <c r="J94">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M94">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.18029222269258616</v>
+      </c>
+      <c r="N94">
+        <f t="shared" ca="1" si="6"/>
+        <v>17.668637823873443</v>
+      </c>
+      <c r="O94">
+        <f t="shared" ca="1" si="7"/>
+        <v>18</v>
+      </c>
+      <c r="P94">
+        <v>91</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -70314,11 +71998,29 @@
         <v>51</v>
       </c>
       <c r="J95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M95">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.9402350853409398</v>
+      </c>
+      <c r="N95">
+        <f t="shared" ca="1" si="6"/>
+        <v>80.860217339320826</v>
+      </c>
+      <c r="O95">
+        <f t="shared" ca="1" si="7"/>
+        <v>81</v>
+      </c>
+      <c r="P95">
+        <v>3</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -70338,11 +72040,29 @@
         <v>20</v>
       </c>
       <c r="J96">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M96">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.53926113566831579</v>
+      </c>
+      <c r="N96">
+        <f t="shared" ca="1" si="6"/>
+        <v>52.847591295494951</v>
+      </c>
+      <c r="O96">
+        <f t="shared" ca="1" si="7"/>
+        <v>53</v>
+      </c>
+      <c r="P96">
+        <v>86</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -70362,11 +72082,29 @@
         <v>20</v>
       </c>
       <c r="J97">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M97">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.59693064864710832</v>
+      </c>
+      <c r="N97">
+        <f t="shared" ca="1" si="6"/>
+        <v>58.499203567416615</v>
+      </c>
+      <c r="O97">
+        <f t="shared" ca="1" si="7"/>
+        <v>59</v>
+      </c>
+      <c r="P97">
+        <v>20</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -70386,11 +72124,29 @@
         <v>51</v>
       </c>
       <c r="J98">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M98">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.15417799019174905</v>
+      </c>
+      <c r="N98">
+        <f t="shared" ca="1" si="6"/>
+        <v>15.109443038791406</v>
+      </c>
+      <c r="O98">
+        <f t="shared" ca="1" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="P98">
+        <v>81</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -70410,11 +72166,29 @@
         <v>20</v>
       </c>
       <c r="J99">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M99">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.32794821805908836</v>
+      </c>
+      <c r="N99">
+        <f t="shared" ca="1" si="6"/>
+        <v>32.138925369790663</v>
+      </c>
+      <c r="O99">
+        <f t="shared" ca="1" si="7"/>
+        <v>33</v>
+      </c>
+      <c r="P99">
+        <v>95</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -70434,11 +72208,29 @@
         <v>20</v>
       </c>
       <c r="J100">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M100">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.66709865676828051</v>
+      </c>
+      <c r="N100">
+        <f t="shared" ca="1" si="6"/>
+        <v>65.375668363291496</v>
+      </c>
+      <c r="O100">
+        <f t="shared" ca="1" si="7"/>
+        <v>66</v>
+      </c>
+      <c r="P100">
+        <v>63</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -70458,11 +72250,29 @@
         <v>20</v>
       </c>
       <c r="J101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M101">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.77030559591399883</v>
+      </c>
+      <c r="N101">
+        <f t="shared" ca="1" si="6"/>
+        <v>72.408726015915889</v>
+      </c>
+      <c r="O101">
+        <f t="shared" ca="1" si="7"/>
+        <v>73</v>
+      </c>
+      <c r="P101">
+        <v>94</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -70482,11 +72292,29 @@
         <v>20</v>
       </c>
       <c r="J102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>88</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M102">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.28192100254329555</v>
+      </c>
+      <c r="N102">
+        <f t="shared" ca="1" si="6"/>
+        <v>24.809048223810009</v>
+      </c>
+      <c r="O102">
+        <f t="shared" ca="1" si="7"/>
+        <v>25</v>
+      </c>
+      <c r="P102">
+        <v>73</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -70506,11 +72334,29 @@
         <v>20</v>
       </c>
       <c r="J103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M103">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.59936328998018584</v>
+      </c>
+      <c r="N103">
+        <f t="shared" ca="1" si="6"/>
+        <v>56.340149258137473</v>
+      </c>
+      <c r="O103">
+        <f t="shared" ca="1" si="7"/>
+        <v>57</v>
+      </c>
+      <c r="P103">
+        <v>50</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -70530,11 +72376,29 @@
         <v>20</v>
       </c>
       <c r="J104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M104">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.7158655287095925E-2</v>
+      </c>
+      <c r="N104">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.612913596987017</v>
+      </c>
+      <c r="O104">
+        <f t="shared" ca="1" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="P104">
+        <v>57</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -70554,11 +72418,29 @@
         <v>20</v>
       </c>
       <c r="J105">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M105">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.97735827873772485</v>
+      </c>
+      <c r="N105">
+        <f t="shared" ca="1" si="6"/>
+        <v>95.781111316297029</v>
+      </c>
+      <c r="O105">
+        <f t="shared" ca="1" si="7"/>
+        <v>96</v>
+      </c>
+      <c r="P105">
+        <v>30</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -70578,11 +72460,29 @@
         <v>51</v>
       </c>
       <c r="J106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M106">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.95899763502920043</v>
+      </c>
+      <c r="N106">
+        <f t="shared" ca="1" si="6"/>
+        <v>92.063772962803242</v>
+      </c>
+      <c r="O106">
+        <f t="shared" ca="1" si="7"/>
+        <v>93</v>
+      </c>
+      <c r="P106">
+        <v>9</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -70602,11 +72502,29 @@
         <v>51</v>
       </c>
       <c r="J107">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M107">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.72347420825577358</v>
+      </c>
+      <c r="N107">
+        <f t="shared" ca="1" si="6"/>
+        <v>70.900472409065813</v>
+      </c>
+      <c r="O107">
+        <f t="shared" ca="1" si="7"/>
+        <v>71</v>
+      </c>
+      <c r="P107">
+        <v>79</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -70626,11 +72544,29 @@
         <v>20</v>
       </c>
       <c r="J108">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M108">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.53077750269149604</v>
+      </c>
+      <c r="N108">
+        <f t="shared" ca="1" si="6"/>
+        <v>52.016195263766612</v>
+      </c>
+      <c r="O108">
+        <f t="shared" ca="1" si="7"/>
+        <v>53</v>
+      </c>
+      <c r="P108">
+        <v>4</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -70650,11 +72586,29 @@
         <v>51</v>
       </c>
       <c r="J109">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M109">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.57684534007306465</v>
+      </c>
+      <c r="N109">
+        <f t="shared" ca="1" si="6"/>
+        <v>56.530843327160333</v>
+      </c>
+      <c r="O109">
+        <f t="shared" ca="1" si="7"/>
+        <v>57</v>
+      </c>
+      <c r="P109">
+        <v>17</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -70674,11 +72628,29 @@
         <v>20</v>
       </c>
       <c r="J110">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M110">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.39072073618753811</v>
+      </c>
+      <c r="N110">
+        <f t="shared" ca="1" si="6"/>
+        <v>38.290632146378734</v>
+      </c>
+      <c r="O110">
+        <f t="shared" ca="1" si="7"/>
+        <v>39</v>
+      </c>
+      <c r="P110">
+        <v>80</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -70698,11 +72670,29 @@
         <v>20</v>
       </c>
       <c r="J111">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="M111">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.46009216190260382</v>
+      </c>
+      <c r="N111">
+        <f t="shared" ca="1" si="6"/>
+        <v>46.009216190260382</v>
+      </c>
+      <c r="O111">
+        <f t="shared" ca="1" si="7"/>
+        <v>47</v>
+      </c>
+      <c r="P111">
+        <v>13</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -70722,11 +72712,29 @@
         <v>20</v>
       </c>
       <c r="J112">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M112">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.30265782166788502</v>
+      </c>
+      <c r="N112">
+        <f t="shared" ca="1" si="6"/>
+        <v>29.660466523452733</v>
+      </c>
+      <c r="O112">
+        <f t="shared" ca="1" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="P112">
+        <v>15</v>
+      </c>
+      <c r="Q112" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -70746,11 +72754,29 @@
         <v>20</v>
       </c>
       <c r="J113">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M113">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.79172851132875666</v>
+      </c>
+      <c r="N113">
+        <f t="shared" ca="1" si="6"/>
+        <v>77.589394110218151</v>
+      </c>
+      <c r="O113">
+        <f t="shared" ca="1" si="7"/>
+        <v>78</v>
+      </c>
+      <c r="P113">
+        <v>21</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -70770,11 +72796,29 @@
         <v>51</v>
       </c>
       <c r="J114">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M114">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.79820303922753755</v>
+      </c>
+      <c r="N114">
+        <f t="shared" ca="1" si="6"/>
+        <v>78.223897844298676</v>
+      </c>
+      <c r="O114">
+        <f t="shared" ca="1" si="7"/>
+        <v>79</v>
+      </c>
+      <c r="P114">
+        <v>2</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -70794,11 +72838,29 @@
         <v>20</v>
       </c>
       <c r="J115">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M115">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.12044405304547146</v>
+      </c>
+      <c r="N115">
+        <f t="shared" ca="1" si="6"/>
+        <v>11.803517198456202</v>
+      </c>
+      <c r="O115">
+        <f t="shared" ca="1" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="P115">
+        <v>78</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -70818,11 +72880,29 @@
         <v>51</v>
       </c>
       <c r="J116">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="M116">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.74256138135476757</v>
+      </c>
+      <c r="N116">
+        <f t="shared" ca="1" si="6"/>
+        <v>74.25613813547676</v>
+      </c>
+      <c r="O116">
+        <f t="shared" ca="1" si="7"/>
+        <v>75</v>
+      </c>
+      <c r="P116">
+        <v>76</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -70842,11 +72922,29 @@
         <v>20</v>
       </c>
       <c r="J117">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M117">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.81060371813171628</v>
+      </c>
+      <c r="N117">
+        <f t="shared" ca="1" si="6"/>
+        <v>79.439164376908195</v>
+      </c>
+      <c r="O117">
+        <f t="shared" ca="1" si="7"/>
+        <v>80</v>
+      </c>
+      <c r="P117">
+        <v>18</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -70866,11 +72964,29 @@
         <v>51</v>
       </c>
       <c r="J118">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M118">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.52242165775746363</v>
+      </c>
+      <c r="N118">
+        <f t="shared" ca="1" si="6"/>
+        <v>51.197322460231433</v>
+      </c>
+      <c r="O118">
+        <f t="shared" ca="1" si="7"/>
+        <v>52</v>
+      </c>
+      <c r="P118">
+        <v>26</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -70890,11 +73006,29 @@
         <v>20</v>
       </c>
       <c r="J119">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M119">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.42888196469282913</v>
+      </c>
+      <c r="N119">
+        <f t="shared" ca="1" si="6"/>
+        <v>42.030432539897255</v>
+      </c>
+      <c r="O119">
+        <f t="shared" ca="1" si="7"/>
+        <v>43</v>
+      </c>
+      <c r="P119">
+        <v>94</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -70914,11 +73048,29 @@
         <v>20</v>
       </c>
       <c r="J120">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M120">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.52048016194144253</v>
+      </c>
+      <c r="N120">
+        <f t="shared" ca="1" si="6"/>
+        <v>51.007055870261368</v>
+      </c>
+      <c r="O120">
+        <f t="shared" ca="1" si="7"/>
+        <v>52</v>
+      </c>
+      <c r="P120">
+        <v>51</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -70938,11 +73090,29 @@
         <v>20</v>
       </c>
       <c r="J121">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M121">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.58556545124799853</v>
+      </c>
+      <c r="N121">
+        <f t="shared" ca="1" si="6"/>
+        <v>57.385414222303858</v>
+      </c>
+      <c r="O121">
+        <f t="shared" ca="1" si="7"/>
+        <v>58</v>
+      </c>
+      <c r="P121">
+        <v>74</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -70962,11 +73132,29 @@
         <v>20</v>
       </c>
       <c r="J122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M122">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.71552904899299263</v>
+      </c>
+      <c r="N122">
+        <f t="shared" ca="1" si="6"/>
+        <v>68.690788703327286</v>
+      </c>
+      <c r="O122">
+        <f t="shared" ca="1" si="7"/>
+        <v>69</v>
+      </c>
+      <c r="P122">
+        <v>54</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -70986,11 +73174,29 @@
         <v>20</v>
       </c>
       <c r="J123">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M123">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.66168311769302912</v>
+      </c>
+      <c r="N123">
+        <f t="shared" ca="1" si="6"/>
+        <v>64.844945533916857</v>
+      </c>
+      <c r="O123">
+        <f t="shared" ca="1" si="7"/>
+        <v>65</v>
+      </c>
+      <c r="P123">
+        <v>17</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -71010,11 +73216,29 @@
         <v>51</v>
       </c>
       <c r="J124">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M124">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.55870394053694206</v>
+      </c>
+      <c r="N124">
+        <f t="shared" ca="1" si="6"/>
+        <v>54.752986172620325</v>
+      </c>
+      <c r="O124">
+        <f t="shared" ca="1" si="7"/>
+        <v>55</v>
+      </c>
+      <c r="P124">
+        <v>59</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -71034,11 +73258,29 @@
         <v>20</v>
       </c>
       <c r="J125">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M125">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.80809184396730305</v>
+      </c>
+      <c r="N125">
+        <f t="shared" ca="1" si="6"/>
+        <v>79.193000708795694</v>
+      </c>
+      <c r="O125">
+        <f t="shared" ca="1" si="7"/>
+        <v>80</v>
+      </c>
+      <c r="P125">
+        <v>68</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -71058,11 +73300,29 @@
         <v>51</v>
       </c>
       <c r="J126">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="M126">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.72463956848823441</v>
+      </c>
+      <c r="N126">
+        <f t="shared" ca="1" si="6"/>
+        <v>72.463956848823443</v>
+      </c>
+      <c r="O126">
+        <f t="shared" ca="1" si="7"/>
+        <v>73</v>
+      </c>
+      <c r="P126">
+        <v>45</v>
+      </c>
+      <c r="Q126" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -71082,11 +73342,29 @@
         <v>20</v>
       </c>
       <c r="J127">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M127">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.43158410209226228</v>
+      </c>
+      <c r="N127">
+        <f t="shared" ca="1" si="6"/>
+        <v>42.2952420050417</v>
+      </c>
+      <c r="O127">
+        <f t="shared" ca="1" si="7"/>
+        <v>43</v>
+      </c>
+      <c r="P127">
+        <v>96</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -71106,11 +73384,29 @@
         <v>51</v>
       </c>
       <c r="J128">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="M128">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.63407769446156237</v>
+      </c>
+      <c r="N128">
+        <f t="shared" ca="1" si="6"/>
+        <v>62.139614057233111</v>
+      </c>
+      <c r="O128">
+        <f t="shared" ca="1" si="7"/>
+        <v>63</v>
+      </c>
+      <c r="P128">
+        <v>89</v>
+      </c>
+      <c r="Q128" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -71130,11 +73426,29 @@
         <v>20</v>
       </c>
       <c r="J129">
-        <f t="shared" ref="J129:J151" si="2">CEILING(E129,2)</f>
+        <f t="shared" ref="J129:J151" si="8">CEILING(E129,2)</f>
         <v>86</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M129">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.59522969420276983</v>
+      </c>
+      <c r="N129">
+        <f t="shared" ca="1" si="6"/>
+        <v>51.189753701438207</v>
+      </c>
+      <c r="O129">
+        <f t="shared" ca="1" si="7"/>
+        <v>52</v>
+      </c>
+      <c r="P129">
+        <v>54</v>
+      </c>
+      <c r="Q129" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -71154,11 +73468,29 @@
         <v>51</v>
       </c>
       <c r="J130">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M130">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.9878182428482174</v>
+      </c>
+      <c r="N130">
+        <f t="shared" ca="1" si="6"/>
+        <v>96.806187799125311</v>
+      </c>
+      <c r="O130">
+        <f t="shared" ca="1" si="7"/>
+        <v>97</v>
+      </c>
+      <c r="P130">
+        <v>91</v>
+      </c>
+      <c r="Q130" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -71178,11 +73510,29 @@
         <v>20</v>
       </c>
       <c r="J131">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M131">
+        <f t="shared" ref="M131:M151" ca="1" si="9">RAND()</f>
+        <v>0.55395056720451918</v>
+      </c>
+      <c r="N131">
+        <f t="shared" ref="N131:N151" ca="1" si="10">M131*E131</f>
+        <v>54.287155586042878</v>
+      </c>
+      <c r="O131">
+        <f t="shared" ref="O131:O151" ca="1" si="11">CEILING(N131,1)</f>
+        <v>55</v>
+      </c>
+      <c r="P131">
+        <v>63</v>
+      </c>
+      <c r="Q131" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -71202,11 +73552,29 @@
         <v>20</v>
       </c>
       <c r="J132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M132">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.13716464493614688</v>
+      </c>
+      <c r="N132">
+        <f t="shared" ca="1" si="10"/>
+        <v>13.167805913870101</v>
+      </c>
+      <c r="O132">
+        <f t="shared" ca="1" si="11"/>
+        <v>14</v>
+      </c>
+      <c r="P132">
+        <v>52</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -71226,11 +73594,29 @@
         <v>20</v>
       </c>
       <c r="J133">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="M133">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.25787316735997323</v>
+      </c>
+      <c r="N133">
+        <f t="shared" ca="1" si="10"/>
+        <v>25.787316735997322</v>
+      </c>
+      <c r="O133">
+        <f t="shared" ca="1" si="11"/>
+        <v>26</v>
+      </c>
+      <c r="P133">
+        <v>79</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -71250,11 +73636,29 @@
         <v>20</v>
       </c>
       <c r="J134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M134">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.38964111153824543</v>
+      </c>
+      <c r="N134">
+        <f t="shared" ca="1" si="10"/>
+        <v>31.950571146136127</v>
+      </c>
+      <c r="O134">
+        <f t="shared" ca="1" si="11"/>
+        <v>32</v>
+      </c>
+      <c r="P134">
+        <v>29</v>
+      </c>
+      <c r="Q134" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -71274,11 +73678,29 @@
         <v>20</v>
       </c>
       <c r="J135">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M135">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.93837396031196374</v>
+      </c>
+      <c r="N135">
+        <f t="shared" ca="1" si="10"/>
+        <v>91.96064811057245</v>
+      </c>
+      <c r="O135">
+        <f t="shared" ca="1" si="11"/>
+        <v>92</v>
+      </c>
+      <c r="P135">
+        <v>84</v>
+      </c>
+      <c r="Q135" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -71298,11 +73720,29 @@
         <v>20</v>
       </c>
       <c r="J136">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M136">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.20295455180436117</v>
+      </c>
+      <c r="N136">
+        <f t="shared" ca="1" si="10"/>
+        <v>19.889546076827394</v>
+      </c>
+      <c r="O136">
+        <f t="shared" ca="1" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="P136">
+        <v>19</v>
+      </c>
+      <c r="Q136" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -71322,11 +73762,29 @@
         <v>20</v>
       </c>
       <c r="J137">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M137">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.86168136405998375</v>
+      </c>
+      <c r="N137">
+        <f t="shared" ca="1" si="10"/>
+        <v>84.444773677878402</v>
+      </c>
+      <c r="O137">
+        <f t="shared" ca="1" si="11"/>
+        <v>85</v>
+      </c>
+      <c r="P137">
+        <v>23</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -71346,11 +73804,29 @@
         <v>20</v>
       </c>
       <c r="J138">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M138">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.908858555478672</v>
+      </c>
+      <c r="N138">
+        <f t="shared" ca="1" si="10"/>
+        <v>89.068138436909862</v>
+      </c>
+      <c r="O138">
+        <f t="shared" ca="1" si="11"/>
+        <v>90</v>
+      </c>
+      <c r="P138">
+        <v>47</v>
+      </c>
+      <c r="Q138" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -71370,11 +73846,29 @@
         <v>20</v>
       </c>
       <c r="J139">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M139">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.40258010340212791</v>
+      </c>
+      <c r="N139">
+        <f t="shared" ca="1" si="10"/>
+        <v>39.452850133408532</v>
+      </c>
+      <c r="O139">
+        <f t="shared" ca="1" si="11"/>
+        <v>40</v>
+      </c>
+      <c r="P139">
+        <v>98</v>
+      </c>
+      <c r="Q139" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -71394,11 +73888,29 @@
         <v>20</v>
       </c>
       <c r="J140">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M140">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.60619416246425561</v>
+      </c>
+      <c r="N140">
+        <f t="shared" ca="1" si="10"/>
+        <v>50.920309646997474</v>
+      </c>
+      <c r="O140">
+        <f t="shared" ca="1" si="11"/>
+        <v>51</v>
+      </c>
+      <c r="P140">
+        <v>27</v>
+      </c>
+      <c r="Q140" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -71418,11 +73930,29 @@
         <v>20</v>
       </c>
       <c r="J141">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M141">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.8365348485917784</v>
+      </c>
+      <c r="N141">
+        <f t="shared" ca="1" si="10"/>
+        <v>81.980415161994287</v>
+      </c>
+      <c r="O141">
+        <f t="shared" ca="1" si="11"/>
+        <v>82</v>
+      </c>
+      <c r="P141">
+        <v>95</v>
+      </c>
+      <c r="Q141" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -71442,11 +73972,29 @@
         <v>51</v>
       </c>
       <c r="J142">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="M142">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.70141006838190167</v>
+      </c>
+      <c r="N142">
+        <f t="shared" ca="1" si="10"/>
+        <v>70.141006838190165</v>
+      </c>
+      <c r="O142">
+        <f t="shared" ca="1" si="11"/>
+        <v>71</v>
+      </c>
+      <c r="P142">
+        <v>32</v>
+      </c>
+      <c r="Q142" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -71466,11 +74014,29 @@
         <v>20</v>
       </c>
       <c r="J143">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="M143">
+        <f t="shared" ca="1" si="9"/>
+        <v>7.7112135672374738E-2</v>
+      </c>
+      <c r="N143">
+        <f t="shared" ca="1" si="10"/>
+        <v>7.7112135672374738</v>
+      </c>
+      <c r="O143">
+        <f t="shared" ca="1" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="P143">
+        <v>28</v>
+      </c>
+      <c r="Q143" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -71490,11 +74056,29 @@
         <v>51</v>
       </c>
       <c r="J144">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M144">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.47627273365217326</v>
+      </c>
+      <c r="N144">
+        <f t="shared" ca="1" si="10"/>
+        <v>46.67472789791298</v>
+      </c>
+      <c r="O144">
+        <f t="shared" ca="1" si="11"/>
+        <v>47</v>
+      </c>
+      <c r="P144">
+        <v>3</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -71514,11 +74098,29 @@
         <v>20</v>
       </c>
       <c r="J145">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M145">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.95874803595040359</v>
+      </c>
+      <c r="N145">
+        <f t="shared" ca="1" si="10"/>
+        <v>93.957307523139548</v>
+      </c>
+      <c r="O145">
+        <f t="shared" ca="1" si="11"/>
+        <v>94</v>
+      </c>
+      <c r="P145">
+        <v>30</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -71538,11 +74140,29 @@
         <v>20</v>
       </c>
       <c r="J146">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M146">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.72111533037612374</v>
+      </c>
+      <c r="N146">
+        <f t="shared" ca="1" si="10"/>
+        <v>70.669302376860131</v>
+      </c>
+      <c r="O146">
+        <f t="shared" ca="1" si="11"/>
+        <v>71</v>
+      </c>
+      <c r="P146">
+        <v>91</v>
+      </c>
+      <c r="Q146" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -71562,11 +74182,29 @@
         <v>51</v>
       </c>
       <c r="J147">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M147">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.20994140931327498</v>
+      </c>
+      <c r="N147">
+        <f t="shared" ca="1" si="10"/>
+        <v>20.574258112700949</v>
+      </c>
+      <c r="O147">
+        <f t="shared" ca="1" si="11"/>
+        <v>21</v>
+      </c>
+      <c r="P147">
+        <v>48</v>
+      </c>
+      <c r="Q147" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -71586,11 +74224,29 @@
         <v>20</v>
       </c>
       <c r="J148">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M148">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.1957394061584149</v>
+      </c>
+      <c r="N148">
+        <f t="shared" ca="1" si="10"/>
+        <v>19.18246180352466</v>
+      </c>
+      <c r="O148">
+        <f t="shared" ca="1" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="P148">
+        <v>13</v>
+      </c>
+      <c r="Q148" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -71610,11 +74266,29 @@
         <v>51</v>
       </c>
       <c r="J149">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M149">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.66196650841225702</v>
+      </c>
+      <c r="N149">
+        <f t="shared" ca="1" si="10"/>
+        <v>64.872717824401192</v>
+      </c>
+      <c r="O149">
+        <f t="shared" ca="1" si="11"/>
+        <v>65</v>
+      </c>
+      <c r="P149">
+        <v>51</v>
+      </c>
+      <c r="Q149" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -71634,11 +74308,29 @@
         <v>20</v>
       </c>
       <c r="J150">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="M150">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.99134447656065394</v>
+      </c>
+      <c r="N150">
+        <f t="shared" ca="1" si="10"/>
+        <v>99.13444765606539</v>
+      </c>
+      <c r="O150">
+        <f t="shared" ca="1" si="11"/>
+        <v>100</v>
+      </c>
+      <c r="P150">
+        <v>22</v>
+      </c>
+      <c r="Q150" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -71658,12 +74350,30 @@
         <v>51</v>
       </c>
       <c r="J151">
-        <f t="shared" si="2"/>
-        <v>98</v>
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="M151">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.21771032302619475</v>
+      </c>
+      <c r="N151">
+        <f t="shared" ca="1" si="10"/>
+        <v>21.335611656567085</v>
+      </c>
+      <c r="O151">
+        <f t="shared" ca="1" si="11"/>
+        <v>22</v>
+      </c>
+      <c r="P151">
+        <v>42</v>
+      </c>
+      <c r="Q151" t="s">
+        <v>1664</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E151"/>
+  <autoFilter ref="A2:E151" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>